<commit_message>
Trabalho 1 - Item 1 - Final
</commit_message>
<xml_diff>
--- a/TabelaItem1.xlsx
+++ b/TabelaItem1.xlsx
@@ -36,9 +36,6 @@
     <t>Valor daconta:</t>
   </si>
   <si>
-    <t>10% GARÇON</t>
-  </si>
-  <si>
     <t>DADOS</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>ENTRADA</t>
+  </si>
+  <si>
+    <t>Subtotal sem 10%</t>
   </si>
 </sst>
 </file>
@@ -747,14 +747,14 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D38"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" style="16" bestFit="1" customWidth="1"/>
   </cols>
@@ -767,7 +767,7 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
       <c r="I1" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J1" s="13"/>
     </row>
@@ -776,12 +776,12 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="28"/>
       <c r="I2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J2" s="14">
         <v>10</v>
@@ -792,12 +792,12 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="28"/>
       <c r="I3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J3" s="14">
         <v>8</v>
@@ -808,12 +808,12 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="28"/>
       <c r="I4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J4" s="14">
         <v>2.5</v>
@@ -824,12 +824,12 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="28"/>
       <c r="I5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" s="14">
         <v>2</v>
@@ -841,7 +841,7 @@
       <c r="C6" s="27"/>
       <c r="D6" s="28"/>
       <c r="I6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J6" s="14">
         <v>4</v>
@@ -856,11 +856,11 @@
         <v>8</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="28"/>
       <c r="I7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J7" s="15">
         <v>3</v>
@@ -870,10 +870,10 @@
       <c r="A8" s="29"/>
       <c r="B8" s="20">
         <f>(B3*J4)+(B4*J5)+(B5*J6)</f>
-        <v>25.5</v>
+        <v>8.5</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="28"/>
     </row>
@@ -881,32 +881,32 @@
       <c r="A9" s="29"/>
       <c r="B9" s="20">
         <f>IF(B8&lt;15,3,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="28"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29"/>
       <c r="B10" s="21">
-        <f>10*(B7+B8+B9)/100</f>
-        <v>3.35</v>
+        <f>(B7+B8+B9)</f>
+        <v>19.5</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D10" s="28"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29"/>
       <c r="B11" s="17">
-        <f>B7+B8+B9+B10</f>
-        <v>36.85</v>
+        <f>B10+((B10*10)/100)</f>
+        <v>21.45</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="28"/>
     </row>
@@ -945,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="28"/>
@@ -955,7 +955,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="28"/>
@@ -965,7 +965,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="28"/>
@@ -981,50 +981,50 @@
         <v>5</v>
       </c>
       <c r="B20" s="19">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="28"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="29"/>
       <c r="B21" s="20">
-        <v>4.5</v>
+        <v>17</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" s="28"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
       <c r="B22" s="20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" s="28"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="29"/>
       <c r="B23" s="21">
-        <v>1.75</v>
+        <v>25</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D23" s="28"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29"/>
       <c r="B24" s="17">
-        <v>19.25</v>
+        <v>27.5</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24" s="28"/>
     </row>
@@ -1045,8 +1045,8 @@
       <c r="B27" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="28"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="26"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
@@ -1063,7 +1063,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29" s="27"/>
       <c r="D29" s="28"/>
@@ -1073,7 +1073,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30" s="27"/>
       <c r="D30" s="28"/>
@@ -1083,7 +1083,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31" s="27"/>
       <c r="D31" s="28"/>
@@ -1099,20 +1099,20 @@
         <v>5</v>
       </c>
       <c r="B33" s="19">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="28"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="29"/>
       <c r="B34" s="20">
-        <v>17</v>
+        <v>25.5</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D34" s="28"/>
     </row>
@@ -1122,27 +1122,27 @@
         <v>0</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D35" s="28"/>
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="29"/>
       <c r="B36" s="21">
-        <v>2.7</v>
+        <v>33.5</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D36" s="28"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="29"/>
       <c r="B37" s="17">
-        <v>29.7</v>
+        <v>36.85</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D37" s="28"/>
     </row>

</xml_diff>